<commit_message>
Update edited session - 2025-11-29T10:06:43.724Z - Cache Bust ID: 17644108037242nskib6hi
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1764408256962_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1764408256962_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>211926</v>
+        <v>221431</v>
       </c>
       <c r="B152" t="str">
         <v>General Surgery</v>
@@ -3433,7 +3433,7 @@
         <v>29/11/2025</v>
       </c>
       <c r="D152" t="str">
-        <v>11:51:08</v>
+        <v>11:51:17</v>
       </c>
       <c r="E152" t="str">
         <v>Manual</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>221431</v>
+        <v>221382</v>
       </c>
       <c r="B153" t="str">
         <v>General Surgery</v>
@@ -3453,7 +3453,7 @@
         <v>29/11/2025</v>
       </c>
       <c r="D153" t="str">
-        <v>11:51:17</v>
+        <v>11:51:27</v>
       </c>
       <c r="E153" t="str">
         <v>Manual</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>221382</v>
+        <v>221519</v>
       </c>
       <c r="B154" t="str">
         <v>General Surgery</v>
@@ -3473,7 +3473,7 @@
         <v>29/11/2025</v>
       </c>
       <c r="D154" t="str">
-        <v>11:51:27</v>
+        <v>11:52:58</v>
       </c>
       <c r="E154" t="str">
         <v>Manual</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>221519</v>
+        <v>221482</v>
       </c>
       <c r="B155" t="str">
         <v>General Surgery</v>
@@ -3493,7 +3493,7 @@
         <v>29/11/2025</v>
       </c>
       <c r="D155" t="str">
-        <v>11:52:58</v>
+        <v>11:53:06</v>
       </c>
       <c r="E155" t="str">
         <v>Manual</v>
@@ -3504,7 +3504,7 @@
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>221482</v>
+        <v>221615</v>
       </c>
       <c r="B156" t="str">
         <v>General Surgery</v>
@@ -3513,38 +3513,18 @@
         <v>29/11/2025</v>
       </c>
       <c r="D156" t="str">
-        <v>11:53:06</v>
+        <v>11:53:13</v>
       </c>
       <c r="E156" t="str">
         <v>Manual</v>
       </c>
       <c r="F156" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="str">
-        <v>221615</v>
-      </c>
-      <c r="B157" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C157" t="str">
-        <v>29/11/2025</v>
-      </c>
-      <c r="D157" t="str">
-        <v>11:53:13</v>
-      </c>
-      <c r="E157" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F157" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F157"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F156"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>